<commit_message>
sync xml with xls file
</commit_message>
<xml_diff>
--- a/SgarbiMix/SgarbiMix.WP7/Data/Sounds.xlsx
+++ b/SgarbiMix/SgarbiMix.WP7/Data/Sounds.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12440"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -20,14 +20,14 @@
 
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
 <connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <connection id="1" name="Sounds" type="4" refreshedVersion="0" background="1">
-    <webPr xml="1" sourceData="1" url="D:\Users\Luca\Documents\Visual Studio 2010\Projects\WPaolo7\SgarbiMix\SgarbiMix.WP7\Data\Sounds.xml" htmlTables="1" htmlFormat="all"/>
+  <connection id="1" name="Sounds" type="4" refreshedVersion="0" background="1" saveData="1">
+    <webPr xml="1" sourceData="1" parsePre="1" consecutive="1" url="D:\Users\Luca\Documents\Visual Studio 2010\Projects\WPaolo7\SgarbiMix\SgarbiMix.Web\SgarbiMix\Sounds.xml" htmlTables="1"/>
   </connection>
 </connections>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="146">
   <si>
     <t>Name</t>
   </si>
@@ -456,6 +456,15 @@
   </si>
   <si>
     <t>e_vaffanculo.wav</t>
+  </si>
+  <si>
+    <t>Quella merda secca</t>
+  </si>
+  <si>
+    <t>quella_m_secca.wav</t>
+  </si>
+  <si>
+    <t>Merda</t>
   </si>
 </sst>
 </file>
@@ -497,7 +506,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normale" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="1">
     <dxf>
@@ -542,9 +551,9 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabella1" displayName="Tabella1" ref="A1:D67" tableType="xml" totalsRowShown="0" connectionId="1">
-  <autoFilter ref="A1:D67"/>
-  <sortState ref="A2:D67">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabella1" displayName="Tabella1" ref="A1:D68" tableType="xml" totalsRowShown="0" connectionId="1">
+  <autoFilter ref="A1:D68"/>
+  <sortState ref="A2:D68">
     <sortCondition ref="C2:C64"/>
     <sortCondition ref="D2:D64"/>
     <sortCondition ref="A2:A64"/>
@@ -568,7 +577,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema di Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -830,20 +839,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D67"/>
+  <dimension ref="A1:D68"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C67" sqref="C67"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="B60" sqref="B60"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="33.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="47.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="31.7265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="43.90625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.54296875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.6328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -857,7 +867,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
@@ -872,7 +882,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
@@ -887,7 +897,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
@@ -902,7 +912,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>6</v>
       </c>
@@ -917,7 +927,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>7</v>
       </c>
@@ -932,14 +942,14 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A7" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="1" t="s">
         <v>118</v>
       </c>
       <c r="D7" s="2">
@@ -947,7 +957,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>8</v>
       </c>
@@ -962,27 +972,27 @@
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
-        <v>138</v>
+        <v>9</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>137</v>
+        <v>63</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>118</v>
       </c>
       <c r="D9" s="2">
         <f>LEN(Tabella1[[#This Row],[Name]])</f>
-        <v>14</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>118</v>
@@ -992,12 +1002,12 @@
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>118</v>
@@ -1007,27 +1017,27 @@
         <v>16</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>118</v>
       </c>
       <c r="D12">
         <f>LEN(Tabella1[[#This Row],[Name]])</f>
-        <v>16</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
-        <v>134</v>
+        <v>13</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>118</v>
@@ -1037,762 +1047,762 @@
         <v>17</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>118</v>
       </c>
       <c r="D14">
         <f>LEN(Tabella1[[#This Row],[Name]])</f>
-        <v>17</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>118</v>
       </c>
       <c r="D15">
         <f>LEN(Tabella1[[#This Row],[Name]])</f>
+        <v>19</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A16" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="D16">
+        <f>LEN(Tabella1[[#This Row],[Name]])</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A17" s="1" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="D16">
-        <f>LEN(Tabella1[[#This Row],[Name]])</f>
-        <v>17</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="1" t="s">
-        <v>14</v>
-      </c>
       <c r="B17" s="1" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="D17">
         <f>LEN(Tabella1[[#This Row],[Name]])</f>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A18" s="1" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="1" t="s">
-        <v>15</v>
-      </c>
       <c r="B18" s="1" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="D18">
         <f>LEN(Tabella1[[#This Row],[Name]])</f>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A19" s="1" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="1" t="s">
-        <v>16</v>
-      </c>
       <c r="B19" s="1" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>119</v>
       </c>
       <c r="D19">
         <f>LEN(Tabella1[[#This Row],[Name]])</f>
-        <v>6</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A20" s="1" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>119</v>
       </c>
       <c r="D20">
         <f>LEN(Tabella1[[#This Row],[Name]])</f>
-        <v>9</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A21" s="1" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>119</v>
       </c>
       <c r="D21">
         <f>LEN(Tabella1[[#This Row],[Name]])</f>
-        <v>9</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A22" s="1" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>119</v>
       </c>
       <c r="D22">
         <f>LEN(Tabella1[[#This Row],[Name]])</f>
-        <v>13</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A23" s="1" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>119</v>
       </c>
       <c r="D23">
         <f>LEN(Tabella1[[#This Row],[Name]])</f>
-        <v>13</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A24" s="1" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="D24">
         <f>LEN(Tabella1[[#This Row],[Name]])</f>
-        <v>21</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A25" s="1" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="D25">
         <f>LEN(Tabella1[[#This Row],[Name]])</f>
-        <v>22</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A26" s="1" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="D26">
         <f>LEN(Tabella1[[#This Row],[Name]])</f>
-        <v>24</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A27" s="1" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="C27" s="1" t="s">
         <v>120</v>
       </c>
       <c r="D27">
         <f>LEN(Tabella1[[#This Row],[Name]])</f>
-        <v>7</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A28" s="1" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="C28" s="1" t="s">
         <v>120</v>
       </c>
       <c r="D28">
         <f>LEN(Tabella1[[#This Row],[Name]])</f>
-        <v>11</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A29" s="1" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="D29">
         <f>LEN(Tabella1[[#This Row],[Name]])</f>
-        <v>14</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A30" s="1" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="D30">
         <f>LEN(Tabella1[[#This Row],[Name]])</f>
         <v>16</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A31" s="1" t="s">
-        <v>28</v>
+        <v>133</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="D31">
         <f>LEN(Tabella1[[#This Row],[Name]])</f>
-        <v>21</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A32" s="1" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="C32" s="1" t="s">
         <v>121</v>
       </c>
       <c r="D32">
         <f>LEN(Tabella1[[#This Row],[Name]])</f>
-        <v>15</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A33" s="1" t="s">
-        <v>30</v>
+        <v>136</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="C33" s="1" t="s">
         <v>121</v>
       </c>
       <c r="D33">
         <f>LEN(Tabella1[[#This Row],[Name]])</f>
-        <v>16</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A34" s="1" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="C34" s="1" t="s">
         <v>121</v>
       </c>
       <c r="D34">
         <f>LEN(Tabella1[[#This Row],[Name]])</f>
-        <v>17</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A35" s="1" t="s">
-        <v>133</v>
+        <v>34</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>87</v>
+        <v>92</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="D35">
         <f>LEN(Tabella1[[#This Row],[Name]])</f>
-        <v>18</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A36" s="1" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="D36">
         <f>LEN(Tabella1[[#This Row],[Name]])</f>
-        <v>22</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A37" s="1" t="s">
-        <v>136</v>
+        <v>36</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="D37">
         <f>LEN(Tabella1[[#This Row],[Name]])</f>
-        <v>24</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A38" s="1" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="D38">
         <f>LEN(Tabella1[[#This Row],[Name]])</f>
-        <v>32</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A39" s="1" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
       <c r="C39" s="1" t="s">
         <v>122</v>
       </c>
       <c r="D39">
         <f>LEN(Tabella1[[#This Row],[Name]])</f>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A40" s="1" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="C40" s="1" t="s">
         <v>122</v>
       </c>
       <c r="D40">
         <f>LEN(Tabella1[[#This Row],[Name]])</f>
-        <v>5</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A41" s="1" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
       <c r="C41" s="1" t="s">
         <v>122</v>
       </c>
       <c r="D41">
         <f>LEN(Tabella1[[#This Row],[Name]])</f>
-        <v>6</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A42" s="1" t="s">
-        <v>37</v>
+        <v>127</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>95</v>
+        <v>128</v>
       </c>
       <c r="C42" s="1" t="s">
         <v>122</v>
       </c>
       <c r="D42">
         <f>LEN(Tabella1[[#This Row],[Name]])</f>
-        <v>9</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A43" s="1" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="C43" s="1" t="s">
         <v>122</v>
       </c>
       <c r="D43">
         <f>LEN(Tabella1[[#This Row],[Name]])</f>
-        <v>11</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A44" s="1" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="C44" s="1" t="s">
         <v>122</v>
       </c>
       <c r="D44">
         <f>LEN(Tabella1[[#This Row],[Name]])</f>
-        <v>14</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A45" s="1" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="C45" s="1" t="s">
         <v>122</v>
       </c>
       <c r="D45">
         <f>LEN(Tabella1[[#This Row],[Name]])</f>
-        <v>14</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A46" s="1" t="s">
-        <v>127</v>
+        <v>44</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>128</v>
+        <v>102</v>
       </c>
       <c r="C46" s="1" t="s">
         <v>122</v>
       </c>
       <c r="D46">
         <f>LEN(Tabella1[[#This Row],[Name]])</f>
-        <v>15</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A47" s="1" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>99</v>
+        <v>104</v>
       </c>
       <c r="C47" s="1" t="s">
         <v>122</v>
       </c>
       <c r="D47">
         <f>LEN(Tabella1[[#This Row],[Name]])</f>
-        <v>16</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A48" s="1" t="s">
-        <v>42</v>
+        <v>132</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="C48" s="1" t="s">
         <v>122</v>
       </c>
       <c r="D48">
         <f>LEN(Tabella1[[#This Row],[Name]])</f>
-        <v>18</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A49" s="1" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>101</v>
+        <v>105</v>
       </c>
       <c r="C49" s="1" t="s">
         <v>122</v>
       </c>
       <c r="D49">
         <f>LEN(Tabella1[[#This Row],[Name]])</f>
-        <v>19</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A50" s="1" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>102</v>
+        <v>106</v>
       </c>
       <c r="C50" s="1" t="s">
         <v>122</v>
       </c>
       <c r="D50">
         <f>LEN(Tabella1[[#This Row],[Name]])</f>
-        <v>20</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A51" s="1" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="C51" s="1" t="s">
         <v>122</v>
       </c>
       <c r="D51">
         <f>LEN(Tabella1[[#This Row],[Name]])</f>
+        <v>28</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A52" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="D52">
+        <f>LEN(Tabella1[[#This Row],[Name]])</f>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A53" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="C53" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="D53">
+        <f>LEN(Tabella1[[#This Row],[Name]])</f>
+        <v>23</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A54" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="D54">
+        <f>LEN(Tabella1[[#This Row],[Name]])</f>
         <v>25</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A52" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="B52" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="C52" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="D52">
-        <f>LEN(Tabella1[[#This Row],[Name]])</f>
-        <v>26</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A53" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="B53" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="C53" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="D53">
-        <f>LEN(Tabella1[[#This Row],[Name]])</f>
-        <v>27</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A54" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="B54" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="C54" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="D54">
-        <f>LEN(Tabella1[[#This Row],[Name]])</f>
-        <v>27</v>
-      </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A55" s="1" t="s">
-        <v>48</v>
+        <v>140</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>107</v>
+        <v>111</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="D55">
-        <f>LEN(Tabella1[[#This Row],[Name]])</f>
-        <v>28</v>
-      </c>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+        <v>123</v>
+      </c>
+      <c r="D55" s="2">
+        <f>LEN(Tabella1[[#This Row],[Name]])</f>
+        <v>34</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A56" s="1" t="s">
-        <v>49</v>
+        <v>130</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>108</v>
+        <v>131</v>
       </c>
       <c r="C56" s="1" t="s">
         <v>123</v>
       </c>
       <c r="D56">
         <f>LEN(Tabella1[[#This Row],[Name]])</f>
-        <v>22</v>
-      </c>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A57" s="1" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="C57" s="1" t="s">
         <v>123</v>
       </c>
       <c r="D57">
         <f>LEN(Tabella1[[#This Row],[Name]])</f>
-        <v>23</v>
-      </c>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A58" s="1" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="C58" s="1" t="s">
         <v>123</v>
       </c>
       <c r="D58">
         <f>LEN(Tabella1[[#This Row],[Name]])</f>
-        <v>25</v>
-      </c>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A59" s="1" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>111</v>
+        <v>137</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>123</v>
+        <v>145</v>
       </c>
       <c r="D59">
         <f>LEN(Tabella1[[#This Row],[Name]])</f>
-        <v>34</v>
-      </c>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A60" s="1" t="s">
-        <v>130</v>
+        <v>134</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>131</v>
+        <v>64</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="D60" s="2">
-        <f>LEN(Tabella1[[#This Row],[Name]])</f>
-        <v>35</v>
-      </c>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+        <v>145</v>
+      </c>
+      <c r="D60">
+        <f>LEN(Tabella1[[#This Row],[Name]])</f>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A61" s="1" t="s">
-        <v>52</v>
+        <v>31</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>112</v>
+        <v>88</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>123</v>
+        <v>145</v>
       </c>
       <c r="D61">
         <f>LEN(Tabella1[[#This Row],[Name]])</f>
-        <v>35</v>
-      </c>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A62" s="1" t="s">
-        <v>53</v>
+        <v>135</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>113</v>
+        <v>66</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>123</v>
+        <v>145</v>
       </c>
       <c r="D62">
         <f>LEN(Tabella1[[#This Row],[Name]])</f>
-        <v>37</v>
-      </c>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A63" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="B63" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="C63" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="D63">
+        <f>LEN(Tabella1[[#This Row],[Name]])</f>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A64" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="B63" s="1" t="s">
+      <c r="B64" s="1" t="s">
         <v>114</v>
-      </c>
-      <c r="C63" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="D63">
-        <f>LEN(Tabella1[[#This Row],[Name]])</f>
-        <v>8</v>
-      </c>
-    </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A64" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="B64" s="1" t="s">
-        <v>115</v>
       </c>
       <c r="C64" s="1" t="s">
         <v>124</v>
@@ -1802,47 +1812,62 @@
         <v>8</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A65" t="s">
-        <v>125</v>
-      </c>
-      <c r="B65" t="s">
-        <v>126</v>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A65" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B65" s="1" t="s">
+        <v>115</v>
       </c>
       <c r="C65" s="1" t="s">
         <v>124</v>
       </c>
       <c r="D65">
         <f>LEN(Tabella1[[#This Row],[Name]])</f>
-        <v>17</v>
-      </c>
-    </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A66" s="1" t="s">
-        <v>139</v>
+        <v>125</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>116</v>
+        <v>126</v>
       </c>
       <c r="C66" s="1" t="s">
         <v>124</v>
       </c>
       <c r="D66">
         <f>LEN(Tabella1[[#This Row],[Name]])</f>
-        <v>23</v>
-      </c>
-    </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A67" s="1" t="s">
-        <v>56</v>
+        <v>139</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C67" s="1" t="s">
         <v>124</v>
       </c>
       <c r="D67">
+        <f>LEN(Tabella1[[#This Row],[Name]])</f>
+        <v>23</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A68" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B68" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="C68" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="D68" s="2">
         <f>LEN(Tabella1[[#This Row],[Name]])</f>
         <v>25</v>
       </c>

</xml_diff>